<commit_message>
exapnd sex and status simplify analysis and add talk
</commit_message>
<xml_diff>
--- a/data/ih-trial_results_20171020.xlsx
+++ b/data/ih-trial_results_20171020.xlsx
@@ -427,16 +427,16 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0.34</v>
+        <v>1.62</v>
       </c>
       <c r="G2">
-        <v>3.49</v>
+        <v>6.89</v>
       </c>
       <c r="H2">
-        <v>2.15</v>
+        <v>7.8</v>
       </c>
       <c r="I2">
-        <v>4.85</v>
+        <v>12.82</v>
       </c>
     </row>
     <row r="3">
@@ -462,16 +462,16 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>3.97</v>
+        <v>5.25</v>
       </c>
       <c r="G3">
-        <v>6.78</v>
+        <v>10.18</v>
       </c>
       <c r="H3">
-        <v>4.27</v>
+        <v>9.92</v>
       </c>
       <c r="I3">
-        <v>4.52</v>
+        <v>12.49</v>
       </c>
     </row>
     <row r="4">
@@ -497,16 +497,16 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>4.05</v>
+        <v>5.33</v>
       </c>
       <c r="G4">
-        <v>5.97</v>
+        <v>9.369999999999999</v>
       </c>
       <c r="H4">
-        <v>5.56</v>
+        <v>11.21</v>
       </c>
       <c r="I4">
-        <v>7.53</v>
+        <v>15.51</v>
       </c>
     </row>
     <row r="5">
@@ -532,16 +532,16 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>6.56</v>
+        <v>7.85</v>
       </c>
       <c r="G5">
-        <v>7.01</v>
+        <v>10.41</v>
       </c>
       <c r="H5">
-        <v>7.07</v>
+        <v>12.72</v>
       </c>
       <c r="I5">
-        <v>6.3</v>
+        <v>14.27</v>
       </c>
     </row>
     <row r="6">
@@ -567,16 +567,16 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <v>6.97</v>
+        <v>8.26</v>
       </c>
       <c r="G6">
-        <v>6.03</v>
+        <v>9.43</v>
       </c>
       <c r="H6">
-        <v>6.24</v>
+        <v>11.89</v>
       </c>
       <c r="I6">
-        <v>6.95</v>
+        <v>14.92</v>
       </c>
     </row>
     <row r="7">
@@ -602,16 +602,16 @@
         <v>3</v>
       </c>
       <c r="F7">
-        <v>9.77</v>
+        <v>11.06</v>
       </c>
       <c r="G7">
-        <v>5.85</v>
+        <v>9.25</v>
       </c>
       <c r="H7">
-        <v>7.71</v>
+        <v>13.36</v>
       </c>
       <c r="I7">
-        <v>10.8</v>
+        <v>18.77</v>
       </c>
     </row>
     <row r="8">
@@ -637,16 +637,16 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>3.04</v>
+        <v>4.33</v>
       </c>
       <c r="G8">
-        <v>7.09</v>
+        <v>10.49</v>
       </c>
       <c r="H8">
-        <v>3.23</v>
+        <v>8.880000000000001</v>
       </c>
       <c r="I8">
-        <v>4.13</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="9">
@@ -672,16 +672,16 @@
         <v>2</v>
       </c>
       <c r="F9">
-        <v>1.14</v>
+        <v>2.43</v>
       </c>
       <c r="G9">
-        <v>5.04</v>
+        <v>8.44</v>
       </c>
       <c r="H9">
-        <v>7.23</v>
+        <v>12.88</v>
       </c>
       <c r="I9">
-        <v>408</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="10">
@@ -707,16 +707,16 @@
         <v>3</v>
       </c>
       <c r="F10">
-        <v>7.19</v>
+        <v>8.48</v>
       </c>
       <c r="G10">
-        <v>5.31</v>
+        <v>8.710000000000001</v>
       </c>
       <c r="H10">
-        <v>2.08</v>
+        <v>7.73</v>
       </c>
       <c r="I10">
-        <v>8.59</v>
+        <v>16.56</v>
       </c>
     </row>
     <row r="11">
@@ -742,16 +742,16 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>7.86</v>
+        <v>9.15</v>
       </c>
       <c r="G11">
-        <v>7.44</v>
+        <v>10.84</v>
       </c>
       <c r="H11">
-        <v>9.029999999999999</v>
+        <v>14.68</v>
       </c>
       <c r="I11">
-        <v>737</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="12">
@@ -777,16 +777,16 @@
         <v>2</v>
       </c>
       <c r="F12">
-        <v>5.78</v>
+        <v>7.06</v>
       </c>
       <c r="G12">
-        <v>9</v>
+        <v>12.4</v>
       </c>
       <c r="H12">
-        <v>8.77</v>
+        <v>14.42</v>
       </c>
       <c r="I12">
-        <v>9.91</v>
+        <v>17.89</v>
       </c>
     </row>
     <row r="13">
@@ -812,16 +812,16 @@
         <v>3</v>
       </c>
       <c r="F13">
-        <v>8.1</v>
+        <v>9.390000000000001</v>
       </c>
       <c r="G13">
-        <v>9.880000000000001</v>
+        <v>13.28</v>
       </c>
       <c r="H13">
-        <v>12.43</v>
+        <v>18.08</v>
       </c>
       <c r="I13">
-        <v>9.949999999999999</v>
+        <v>17.92</v>
       </c>
     </row>
     <row r="14">
@@ -847,16 +847,16 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>1.72</v>
+        <v>3</v>
       </c>
       <c r="G14">
-        <v>8.68</v>
+        <v>12.08</v>
       </c>
       <c r="H14">
-        <v>4.21</v>
+        <v>9.859999999999999</v>
       </c>
       <c r="I14">
-        <v>0.93</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="15">
@@ -882,16 +882,16 @@
         <v>2</v>
       </c>
       <c r="F15">
-        <v>5.49</v>
+        <v>6.78</v>
       </c>
       <c r="G15">
-        <v>8.390000000000001</v>
+        <v>11.79</v>
       </c>
       <c r="H15">
-        <v>3.87</v>
+        <v>9.52</v>
       </c>
       <c r="I15">
-        <v>3.68</v>
+        <v>11.65</v>
       </c>
     </row>
     <row r="16">
@@ -917,16 +917,16 @@
         <v>3</v>
       </c>
       <c r="F16">
-        <v>4.2</v>
+        <v>5.48</v>
       </c>
       <c r="G16">
-        <v>7.51</v>
+        <v>10.91</v>
       </c>
       <c r="H16">
-        <v>7.36</v>
+        <v>13.01</v>
       </c>
       <c r="I16">
-        <v>6.58</v>
+        <v>14.55</v>
       </c>
     </row>
     <row r="17">
@@ -952,16 +952,16 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>4.89</v>
+        <v>6.17</v>
       </c>
       <c r="G17">
-        <v>7.46</v>
+        <v>10.86</v>
       </c>
       <c r="H17">
-        <v>9.69</v>
+        <v>15.34</v>
       </c>
       <c r="I17">
-        <v>8.140000000000001</v>
+        <v>16.11</v>
       </c>
     </row>
     <row r="18">
@@ -987,16 +987,16 @@
         <v>2</v>
       </c>
       <c r="F18">
-        <v>604</v>
+        <v>732</v>
       </c>
       <c r="G18">
-        <v>8.91</v>
+        <v>12.31</v>
       </c>
       <c r="H18">
-        <v>6.31</v>
+        <v>11.96</v>
       </c>
       <c r="I18">
-        <v>9.630000000000001</v>
+        <v>17.6</v>
       </c>
     </row>
     <row r="19">
@@ -1022,16 +1022,16 @@
         <v>3</v>
       </c>
       <c r="F19">
-        <v>8.279999999999999</v>
+        <v>9.57</v>
       </c>
       <c r="G19">
-        <v>9.630000000000001</v>
+        <v>13.03</v>
       </c>
       <c r="H19">
-        <v>8.24</v>
+        <v>13.89</v>
       </c>
       <c r="I19">
-        <v>8.01</v>
+        <v>15.98</v>
       </c>
     </row>
     <row r="20">
@@ -1057,16 +1057,16 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <v>7.94</v>
+        <v>9.220000000000001</v>
       </c>
       <c r="G20">
-        <v>2.79</v>
+        <v>6.19</v>
       </c>
       <c r="H20">
-        <v>1.85</v>
+        <v>7.5</v>
       </c>
       <c r="I20">
-        <v>5.84</v>
+        <v>13.81</v>
       </c>
     </row>
     <row r="21">
@@ -1092,16 +1092,16 @@
         <v>2</v>
       </c>
       <c r="F21">
-        <v>2.71</v>
+        <v>3.99</v>
       </c>
       <c r="G21">
-        <v>1.99</v>
+        <v>5.39</v>
       </c>
       <c r="H21">
-        <v>7.85</v>
+        <v>13.5</v>
       </c>
       <c r="I21">
-        <v>3.77</v>
+        <v>11.74</v>
       </c>
     </row>
     <row r="22">
@@ -1127,16 +1127,16 @@
         <v>3</v>
       </c>
       <c r="F22">
-        <v>7.29</v>
+        <v>8.58</v>
       </c>
       <c r="G22">
-        <v>4.91</v>
+        <v>8.31</v>
       </c>
       <c r="H22">
-        <v>7.48</v>
+        <v>13.13</v>
       </c>
       <c r="I22">
-        <v>6.12</v>
+        <v>14.09</v>
       </c>
     </row>
     <row r="23">
@@ -1162,16 +1162,16 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <v>9.07</v>
+        <v>10.35</v>
       </c>
       <c r="G23">
-        <v>4.72</v>
+        <v>8.119999999999999</v>
       </c>
       <c r="H23">
-        <v>10.28</v>
+        <v>15.93</v>
       </c>
       <c r="I23">
-        <v>6.62</v>
+        <v>14.6</v>
       </c>
     </row>
     <row r="24">
@@ -1197,16 +1197,16 @@
         <v>2</v>
       </c>
       <c r="F24">
-        <v>6.53</v>
+        <v>7.82</v>
       </c>
       <c r="G24">
-        <v>8.49</v>
+        <v>11.89</v>
       </c>
       <c r="H24">
-        <v>9.640000000000001</v>
+        <v>15.29</v>
       </c>
       <c r="I24">
-        <v>8.59</v>
+        <v>16.56</v>
       </c>
     </row>
     <row r="25">
@@ -1232,16 +1232,16 @@
         <v>3</v>
       </c>
       <c r="F25">
-        <v>4.27</v>
+        <v>5.56</v>
       </c>
       <c r="G25">
-        <v>10.17</v>
+        <v>13.57</v>
       </c>
       <c r="H25">
-        <v>10.43</v>
+        <v>16.08</v>
       </c>
       <c r="I25">
-        <v>7.82</v>
+        <v>15.79</v>
       </c>
     </row>
     <row r="26">
@@ -1267,16 +1267,16 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <v>5.95</v>
+        <v>7.24</v>
       </c>
       <c r="G26">
-        <v>6.25</v>
+        <v>9.65</v>
       </c>
       <c r="H26">
-        <v>6.13</v>
+        <v>11.78</v>
       </c>
       <c r="I26">
-        <v>8.07</v>
+        <v>16.04</v>
       </c>
     </row>
     <row r="27">
@@ -1302,16 +1302,16 @@
         <v>2</v>
       </c>
       <c r="F27">
-        <v>5.31</v>
+        <v>6.6</v>
       </c>
       <c r="G27">
-        <v>0.4</v>
+        <v>3.8</v>
       </c>
       <c r="H27">
-        <v>5.29</v>
+        <v>10.94</v>
       </c>
       <c r="I27">
-        <v>4.78</v>
+        <v>12.75</v>
       </c>
     </row>
     <row r="28">
@@ -1337,16 +1337,16 @@
         <v>3</v>
       </c>
       <c r="F28">
-        <v>4.58</v>
+        <v>5.86</v>
       </c>
       <c r="G28">
-        <v>6.61</v>
+        <v>10.01</v>
       </c>
       <c r="H28">
-        <v>6.39</v>
+        <v>12.04</v>
       </c>
       <c r="I28">
-        <v>7.04</v>
+        <v>15.01</v>
       </c>
     </row>
     <row r="29">
@@ -1372,16 +1372,16 @@
         <v>1</v>
       </c>
       <c r="F29">
-        <v>11.34</v>
+        <v>12.63</v>
       </c>
       <c r="G29">
-        <v>5.72</v>
+        <v>9.119999999999999</v>
       </c>
       <c r="H29">
-        <v>9.869999999999999</v>
+        <v>15.52</v>
       </c>
       <c r="I29">
-        <v>9.25</v>
+        <v>17.22</v>
       </c>
     </row>
     <row r="30">
@@ -1407,16 +1407,16 @@
         <v>2</v>
       </c>
       <c r="F30">
-        <v>7.01</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="G30">
-        <v>10.82</v>
+        <v>14.22</v>
       </c>
       <c r="H30">
-        <v>11.03</v>
+        <v>16.68</v>
       </c>
       <c r="I30">
-        <v>10</v>
+        <v>17.97</v>
       </c>
     </row>
     <row r="31">
@@ -1442,16 +1442,16 @@
         <v>3</v>
       </c>
       <c r="F31">
-        <v>10.97</v>
+        <v>12.26</v>
       </c>
       <c r="G31">
-        <v>7.25</v>
+        <v>10.65</v>
       </c>
       <c r="H31">
-        <v>9.17</v>
+        <v>14.82</v>
       </c>
       <c r="I31">
-        <v>7.44</v>
+        <v>15.41</v>
       </c>
     </row>
     <row r="32">
@@ -1477,16 +1477,16 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <v>4.07</v>
+        <v>5.36</v>
       </c>
       <c r="G32">
-        <v>1.84</v>
+        <v>5.24</v>
       </c>
       <c r="H32">
-        <v>3.41</v>
+        <v>9.07</v>
       </c>
       <c r="I32">
-        <v>4.67</v>
+        <v>12.64</v>
       </c>
     </row>
     <row r="33">
@@ -1512,16 +1512,16 @@
         <v>2</v>
       </c>
       <c r="F33">
-        <v>3.72</v>
+        <v>5</v>
       </c>
       <c r="G33">
-        <v>0.48</v>
+        <v>3.88</v>
       </c>
       <c r="H33">
-        <v>4.88</v>
+        <v>10.53</v>
       </c>
       <c r="I33">
-        <v>6.39</v>
+        <v>14.36</v>
       </c>
     </row>
     <row r="34">
@@ -1547,16 +1547,16 @@
         <v>3</v>
       </c>
       <c r="F34">
-        <v>2.3</v>
+        <v>3.59</v>
       </c>
       <c r="G34">
-        <v>7.09</v>
+        <v>10.49</v>
       </c>
       <c r="H34">
-        <v>3.37</v>
+        <v>9.02</v>
       </c>
       <c r="I34">
-        <v>6.24</v>
+        <v>14.22</v>
       </c>
     </row>
     <row r="35">
@@ -1582,16 +1582,16 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <v>5.19</v>
+        <v>6.48</v>
       </c>
       <c r="G35">
-        <v>6.52</v>
+        <v>9.92</v>
       </c>
       <c r="H35">
-        <v>723</v>
+        <v>1288</v>
       </c>
       <c r="I35">
-        <v>10.86</v>
+        <v>18.83</v>
       </c>
     </row>
     <row r="36">
@@ -1617,16 +1617,16 @@
         <v>2</v>
       </c>
       <c r="F36">
-        <v>5.77</v>
+        <v>7.05</v>
       </c>
       <c r="G36">
-        <v>776</v>
+        <v>1116</v>
       </c>
       <c r="H36">
-        <v>4.26</v>
+        <v>9.91</v>
       </c>
       <c r="I36">
-        <v>9.17</v>
+        <v>17.14</v>
       </c>
     </row>
     <row r="37">
@@ -1652,16 +1652,16 @@
         <v>3</v>
       </c>
       <c r="F37">
-        <v>8.27</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="G37">
-        <v>9.380000000000001</v>
+        <v>12.78</v>
       </c>
       <c r="H37">
-        <v>6.47</v>
+        <v>12.12</v>
       </c>
       <c r="I37">
-        <v>10.51</v>
+        <v>18.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>